<commit_message>
Draft changes and added yields to heatmap
</commit_message>
<xml_diff>
--- a/draft/fig2/heatmap.xlsx
+++ b/draft/fig2/heatmap.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21140" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="2620" yWindow="0" windowWidth="33740" windowHeight="21140" tabRatio="500" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,6 +12,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
     <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
+    <sheet name="Sheet1 (2)" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="221">
   <si>
     <t>sample</t>
   </si>
@@ -680,16 +681,23 @@
   </si>
   <si>
     <t>WT</t>
+  </si>
+  <si>
+    <t>`</t>
+  </si>
+  <si>
+    <t>BglB</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode=";;;"/>
+    <numFmt numFmtId="165" formatCode=";;"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -747,6 +755,27 @@
       <color theme="1"/>
       <name val="Myriad Pro"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Menlo"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Helvetica"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="95"/>
+      <color theme="1"/>
+      <name val="Myriad Pro"/>
+    </font>
+    <font>
+      <sz val="144"/>
+      <color theme="1"/>
+      <name val="Myriad Pro"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -774,7 +803,7 @@
       </diagonal>
     </border>
   </borders>
-  <cellStyleXfs count="37">
+  <cellStyleXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -812,8 +841,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -831,8 +868,18 @@
     <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="37">
+  <cellStyles count="45">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -851,6 +898,10 @@
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -869,9 +920,140 @@
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="11">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -3209,7 +3391,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
+    <sheetView topLeftCell="A71" workbookViewId="0">
       <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
@@ -7349,4 +7531,1757 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="B1:Y104"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A81" zoomScale="16" zoomScaleNormal="16" zoomScalePageLayoutView="16" workbookViewId="0">
+      <selection activeCell="U64" sqref="U64"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="180" customHeight="1" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="193" style="5" customWidth="1"/>
+    <col min="2" max="2" width="30" style="13" customWidth="1"/>
+    <col min="3" max="5" width="30" style="6" customWidth="1"/>
+    <col min="6" max="6" width="1.33203125" style="6" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" style="15"/>
+    <col min="8" max="8" width="69.6640625" style="16" customWidth="1"/>
+    <col min="9" max="9" width="27.33203125" style="5" customWidth="1"/>
+    <col min="10" max="10" width="82.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="10.83203125" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:25" ht="180" customHeight="1">
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="3"/>
+    </row>
+    <row r="2" spans="2:25" ht="180" customHeight="1">
+      <c r="B2" s="11">
+        <v>0.6</v>
+      </c>
+      <c r="C2" s="6">
+        <v>-0.44130228669316729</v>
+      </c>
+      <c r="D2" s="6">
+        <v>-0.20464671950873381</v>
+      </c>
+      <c r="E2" s="6">
+        <v>-0.64594642082365272</v>
+      </c>
+      <c r="G2" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="I2" s="6">
+        <v>1</v>
+      </c>
+      <c r="J2" s="14">
+        <v>1</v>
+      </c>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+    </row>
+    <row r="3" spans="2:25" ht="180" customHeight="1">
+      <c r="B3" s="11">
+        <v>0.83</v>
+      </c>
+      <c r="C3" s="6">
+        <v>-0.75893154417661002</v>
+      </c>
+      <c r="D3" s="6">
+        <v>-0.43432080663704675</v>
+      </c>
+      <c r="E3" s="6">
+        <v>-1.1932511226035434</v>
+      </c>
+      <c r="G3" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="I3" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="J3" s="14"/>
+    </row>
+    <row r="4" spans="2:25" ht="180" customHeight="1">
+      <c r="B4" s="11">
+        <v>0.65</v>
+      </c>
+      <c r="C4" s="6">
+        <v>-0.13959423549425587</v>
+      </c>
+      <c r="D4" s="6">
+        <v>-0.1527038520172006</v>
+      </c>
+      <c r="E4" s="6">
+        <v>-0.29229837696333849</v>
+      </c>
+      <c r="G4" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="I4" s="6">
+        <v>0.25</v>
+      </c>
+      <c r="J4" s="14"/>
+    </row>
+    <row r="5" spans="2:25" ht="180" customHeight="1">
+      <c r="B5" s="11">
+        <v>1.01</v>
+      </c>
+      <c r="C5" s="6">
+        <v>-1.8056412756359386E-2</v>
+      </c>
+      <c r="D5" s="6">
+        <v>-0.55536449936182253</v>
+      </c>
+      <c r="E5" s="6">
+        <v>-0.57341814749162889</v>
+      </c>
+      <c r="G5" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="I5" s="6">
+        <v>0</v>
+      </c>
+      <c r="J5" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:25" ht="180" customHeight="1">
+      <c r="B6" s="11">
+        <v>0.17</v>
+      </c>
+      <c r="C6" s="6">
+        <v>-0.65198603885148021</v>
+      </c>
+      <c r="D6" s="6">
+        <v>-0.78650332474840923</v>
+      </c>
+      <c r="E6" s="6">
+        <v>-1.4384859308548541</v>
+      </c>
+      <c r="G6" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="I6" s="6">
+        <v>-1.25</v>
+      </c>
+      <c r="J6" s="14"/>
+    </row>
+    <row r="7" spans="2:25" ht="180" customHeight="1">
+      <c r="B7" s="11">
+        <v>0.26</v>
+      </c>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="6">
+        <v>-4.7575225530421061</v>
+      </c>
+      <c r="G7" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="I7" s="6">
+        <v>-2.5</v>
+      </c>
+      <c r="J7" s="14"/>
+    </row>
+    <row r="8" spans="2:25" ht="180" customHeight="1">
+      <c r="B8" s="11">
+        <v>0.43</v>
+      </c>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="6">
+        <v>-4.331553820769825</v>
+      </c>
+      <c r="G8" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="I8" s="6">
+        <v>-5</v>
+      </c>
+      <c r="J8" s="14">
+        <v>-5</v>
+      </c>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9"/>
+      <c r="N8" s="9"/>
+    </row>
+    <row r="9" spans="2:25" ht="180" customHeight="1">
+      <c r="B9" s="11">
+        <v>0.4</v>
+      </c>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="6">
+        <v>-4.53567380342575</v>
+      </c>
+      <c r="G9" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="9"/>
+      <c r="N9" s="9"/>
+    </row>
+    <row r="10" spans="2:25" ht="180" customHeight="1">
+      <c r="B10" s="11">
+        <v>0.1</v>
+      </c>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="G10" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="K10" s="9"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="9"/>
+      <c r="N10" s="9"/>
+    </row>
+    <row r="11" spans="2:25" ht="180" customHeight="1">
+      <c r="B11" s="11">
+        <v>0.97</v>
+      </c>
+      <c r="C11" s="6">
+        <v>-0.10949552795352258</v>
+      </c>
+      <c r="D11" s="6">
+        <v>-0.20464671950873381</v>
+      </c>
+      <c r="E11" s="6">
+        <v>-0.31413959689263216</v>
+      </c>
+      <c r="G11" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="K11" s="9"/>
+      <c r="L11" s="9"/>
+      <c r="M11" s="9"/>
+      <c r="N11" s="9"/>
+    </row>
+    <row r="12" spans="2:25" ht="180" customHeight="1">
+      <c r="B12" s="11">
+        <v>0.44</v>
+      </c>
+      <c r="C12" s="6">
+        <v>-0.15899179049465806</v>
+      </c>
+      <c r="D12" s="6">
+        <v>-2.618009729223969E-2</v>
+      </c>
+      <c r="E12" s="6">
+        <v>-0.18516993693403894</v>
+      </c>
+      <c r="G12" s="15" t="s">
+        <v>124</v>
+      </c>
+      <c r="Y12" s="5" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="13" spans="2:25" ht="180" customHeight="1">
+      <c r="B13" s="11">
+        <v>0.1</v>
+      </c>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="G13" s="15" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="14" spans="2:25" ht="180" customHeight="1">
+      <c r="B14" s="11">
+        <v>0.49</v>
+      </c>
+      <c r="C14" s="6">
+        <v>-1.9081901974049575E-2</v>
+      </c>
+      <c r="D14" s="6">
+        <v>-0.11491529112780086</v>
+      </c>
+      <c r="E14" s="6">
+        <v>-0.13399760761628876</v>
+      </c>
+      <c r="G14" s="15" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="15" spans="2:25" ht="180" customHeight="1">
+      <c r="B15" s="11">
+        <v>1.03</v>
+      </c>
+      <c r="C15" s="6">
+        <v>7.8853600251697298E-2</v>
+      </c>
+      <c r="D15" s="6">
+        <v>-0.31349863622357899</v>
+      </c>
+      <c r="E15" s="6">
+        <v>-0.23464380776176874</v>
+      </c>
+      <c r="G15" s="15" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="16" spans="2:25" ht="180" customHeight="1">
+      <c r="B16" s="11">
+        <v>1.02</v>
+      </c>
+      <c r="C16" s="6">
+        <v>-2.6676986640602443</v>
+      </c>
+      <c r="D16" s="6">
+        <v>-0.65368075584970842</v>
+      </c>
+      <c r="E16" s="6">
+        <v>-3.320829955378052</v>
+      </c>
+      <c r="G16" s="15" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" ht="180" customHeight="1">
+      <c r="B17" s="11">
+        <v>1.21</v>
+      </c>
+      <c r="C17" s="6">
+        <v>-0.79111622754801125</v>
+      </c>
+      <c r="D17" s="6">
+        <v>-0.46716971825197828</v>
+      </c>
+      <c r="E17" s="6">
+        <v>-1.2582938287584953</v>
+      </c>
+      <c r="G17" s="15" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" ht="180" customHeight="1">
+      <c r="B18" s="11">
+        <v>0</v>
+      </c>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="G18" s="15" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" ht="180" customHeight="1">
+      <c r="B19" s="11">
+        <v>1</v>
+      </c>
+      <c r="C19" s="6">
+        <v>-1.021656269215161</v>
+      </c>
+      <c r="D19" s="6">
+        <v>-1.238557625334932</v>
+      </c>
+      <c r="E19" s="6">
+        <v>-2.2601321150244402</v>
+      </c>
+      <c r="G19" s="15" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" ht="180" customHeight="1">
+      <c r="B20" s="11">
+        <v>0.16</v>
+      </c>
+      <c r="C20" s="6">
+        <v>-0.27251026637898512</v>
+      </c>
+      <c r="D20" s="6">
+        <v>-0.49501864699065856</v>
+      </c>
+      <c r="E20" s="6">
+        <v>-0.76752428074579182</v>
+      </c>
+      <c r="G20" s="15" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" ht="180" customHeight="1">
+      <c r="B21" s="11">
+        <v>0.78</v>
+      </c>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="15" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" ht="180" customHeight="1">
+      <c r="B22" s="11">
+        <v>0.23</v>
+      </c>
+      <c r="C22" s="6">
+        <v>-2.2836944333314992</v>
+      </c>
+      <c r="D22" s="6">
+        <v>-9.7752485594076788E-2</v>
+      </c>
+      <c r="E22" s="6">
+        <v>-2.381554277909903</v>
+      </c>
+      <c r="G22" s="15" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" ht="180" customHeight="1">
+      <c r="B23" s="11">
+        <v>1.42</v>
+      </c>
+      <c r="C23" s="6">
+        <v>-2.957749106970553E-3</v>
+      </c>
+      <c r="D23" s="6">
+        <v>0.17273113024841447</v>
+      </c>
+      <c r="E23" s="6">
+        <v>0.16977422353168681</v>
+      </c>
+      <c r="G23" s="15" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" ht="180" customHeight="1">
+      <c r="B24" s="11">
+        <v>0.74</v>
+      </c>
+      <c r="C24" s="6">
+        <v>-2.1203774623122467</v>
+      </c>
+      <c r="D24" s="6">
+        <v>-0.36373973235133961</v>
+      </c>
+      <c r="E24" s="6">
+        <v>-2.4841354129104225</v>
+      </c>
+      <c r="G24" s="15" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" ht="180" customHeight="1">
+      <c r="B25" s="11">
+        <v>0.9</v>
+      </c>
+      <c r="C25" s="6">
+        <v>-1.8672710189654482</v>
+      </c>
+      <c r="D25" s="6">
+        <v>-0.47003635890358142</v>
+      </c>
+      <c r="E25" s="6">
+        <v>-2.3375668045523486</v>
+      </c>
+      <c r="G25" s="15" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" ht="180" customHeight="1">
+      <c r="B26" s="11">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C26" s="6">
+        <v>-1.5348325590498428</v>
+      </c>
+      <c r="D26" s="6">
+        <v>-2.2192057497195883E-2</v>
+      </c>
+      <c r="E26" s="6">
+        <v>-1.5570368550412756</v>
+      </c>
+      <c r="G26" s="15" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" ht="180" customHeight="1">
+      <c r="B27" s="11">
+        <v>0.42</v>
+      </c>
+      <c r="C27" s="6">
+        <v>-3.6454222693490919</v>
+      </c>
+      <c r="D27" s="6">
+        <v>0.70748585525854857</v>
+      </c>
+      <c r="E27" s="6">
+        <v>-2.9379786175002378</v>
+      </c>
+      <c r="G27" s="15" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" ht="180" customHeight="1">
+      <c r="B28" s="11">
+        <v>0.18</v>
+      </c>
+      <c r="C28" s="6">
+        <v>-1.5232063910762652</v>
+      </c>
+      <c r="D28" s="6">
+        <v>0.31386722036915371</v>
+      </c>
+      <c r="E28" s="6">
+        <v>-1.2093379424969983</v>
+      </c>
+      <c r="G28" s="15" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" ht="180" customHeight="1">
+      <c r="B29" s="11">
+        <v>0.38</v>
+      </c>
+      <c r="C29" s="6">
+        <v>-0.26611675159850989</v>
+      </c>
+      <c r="D29" s="6">
+        <v>-0.45254562674324594</v>
+      </c>
+      <c r="E29" s="6">
+        <v>-0.71866405148234058</v>
+      </c>
+      <c r="G29" s="15" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" ht="180" customHeight="1">
+      <c r="B30" s="11">
+        <v>0.94</v>
+      </c>
+      <c r="C30" s="6">
+        <v>-0.24402172856754767</v>
+      </c>
+      <c r="D30" s="6">
+        <v>1.9842126273831084E-2</v>
+      </c>
+      <c r="E30" s="6">
+        <v>-0.22417847748706432</v>
+      </c>
+      <c r="G30" s="15" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" ht="180" customHeight="1">
+      <c r="B31" s="11">
+        <v>0.38</v>
+      </c>
+      <c r="C31" s="6">
+        <v>-0.34114721887196353</v>
+      </c>
+      <c r="D31" s="6">
+        <v>0.18546795165134711</v>
+      </c>
+      <c r="E31" s="6">
+        <v>-0.15567976326000821</v>
+      </c>
+      <c r="G31" s="15" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7" ht="180" customHeight="1">
+      <c r="B32" s="11">
+        <v>1.07</v>
+      </c>
+      <c r="C32" s="6">
+        <v>-3.9578730291002895E-2</v>
+      </c>
+      <c r="D32" s="6">
+        <v>-0.33351574974546616</v>
+      </c>
+      <c r="E32" s="6">
+        <v>-0.37309147590459624</v>
+      </c>
+      <c r="G32" s="15" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" ht="180" customHeight="1">
+      <c r="B33" s="11">
+        <v>0.86</v>
+      </c>
+      <c r="C33" s="6">
+        <v>-4.2819748928835555E-2</v>
+      </c>
+      <c r="D33" s="6">
+        <v>0.15671278046287229</v>
+      </c>
+      <c r="E33" s="6">
+        <v>0.11389469349622505</v>
+      </c>
+      <c r="G33" s="15" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" ht="180" customHeight="1">
+      <c r="B34" s="11">
+        <v>0.77</v>
+      </c>
+      <c r="C34" s="6">
+        <v>-0.20215928189039678</v>
+      </c>
+      <c r="D34" s="6">
+        <v>-7.9883419978926895E-2</v>
+      </c>
+      <c r="E34" s="6">
+        <v>-0.2820402294659905</v>
+      </c>
+      <c r="G34" s="15" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" ht="180" customHeight="1">
+      <c r="B35" s="11">
+        <v>0.95</v>
+      </c>
+      <c r="C35" s="6">
+        <v>-0.12037746231224666</v>
+      </c>
+      <c r="D35" s="6">
+        <v>-0.16209436882327033</v>
+      </c>
+      <c r="E35" s="6">
+        <v>-0.28247153633544286</v>
+      </c>
+      <c r="G35" s="15" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" ht="180" customHeight="1">
+      <c r="B36" s="11">
+        <v>0.96</v>
+      </c>
+      <c r="C36" s="6">
+        <v>4.7424649928137885E-2</v>
+      </c>
+      <c r="D36" s="6">
+        <v>-6.4893954947219612E-2</v>
+      </c>
+      <c r="E36" s="6">
+        <v>-1.7467927052276622E-2</v>
+      </c>
+      <c r="G36" s="15" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7" ht="180" customHeight="1">
+      <c r="B37" s="11">
+        <v>0.25</v>
+      </c>
+      <c r="C37" s="6">
+        <v>-0.89337382152965361</v>
+      </c>
+      <c r="D37" s="6">
+        <v>-0.17298813490778997</v>
+      </c>
+      <c r="E37" s="6">
+        <v>-1.0663526189105026</v>
+      </c>
+      <c r="G37" s="15" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7" ht="180" customHeight="1">
+      <c r="B38" s="11">
+        <v>1.17</v>
+      </c>
+      <c r="C38" s="6">
+        <v>2.9438871388719701E-2</v>
+      </c>
+      <c r="D38" s="6">
+        <v>5.0894467044324543E-3</v>
+      </c>
+      <c r="E38" s="6">
+        <v>3.4530441518240806E-2</v>
+      </c>
+      <c r="G38" s="15" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7" ht="180" customHeight="1">
+      <c r="B39" s="11">
+        <v>0.98</v>
+      </c>
+      <c r="C39" s="6">
+        <v>-0.27993428445819246</v>
+      </c>
+      <c r="D39" s="6">
+        <v>-0.10177375952700096</v>
+      </c>
+      <c r="E39" s="6">
+        <v>-0.38170658178027139</v>
+      </c>
+      <c r="G39" s="15" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7" ht="180" customHeight="1">
+      <c r="B40" s="11">
+        <v>0.47</v>
+      </c>
+      <c r="C40" s="6">
+        <v>-0.64759918860336629</v>
+      </c>
+      <c r="D40" s="6">
+        <v>-0.18416750331787357</v>
+      </c>
+      <c r="E40" s="6">
+        <v>-0.8317636741596619</v>
+      </c>
+      <c r="G40" s="15" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="41" spans="2:7" ht="180" customHeight="1">
+      <c r="B41" s="11">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="C41" s="6">
+        <v>-0.85654715357367506</v>
+      </c>
+      <c r="D41" s="6">
+        <v>8.4411004591533612E-4</v>
+      </c>
+      <c r="E41" s="6">
+        <v>-0.85570110914833108</v>
+      </c>
+      <c r="G41" s="15" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="42" spans="2:7" ht="180" customHeight="1">
+      <c r="B42" s="11">
+        <v>0.62</v>
+      </c>
+      <c r="C42" s="6">
+        <v>-0.3389972417984044</v>
+      </c>
+      <c r="D42" s="6">
+        <v>-0.30102999566398103</v>
+      </c>
+      <c r="E42" s="6">
+        <v>-0.64003029860167082</v>
+      </c>
+      <c r="G42" s="15" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="43" spans="2:7" ht="180" customHeight="1">
+      <c r="B43" s="11">
+        <v>0.73</v>
+      </c>
+      <c r="C43" s="6">
+        <v>-0.20846493867964222</v>
+      </c>
+      <c r="D43" s="6">
+        <v>-8.4072788302884227E-2</v>
+      </c>
+      <c r="E43" s="6">
+        <v>-0.29253649877241283</v>
+      </c>
+      <c r="G43" s="15" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="44" spans="2:7" ht="180" customHeight="1">
+      <c r="B44" s="11">
+        <v>0.7</v>
+      </c>
+      <c r="C44" s="6">
+        <v>-1.8782664032669114</v>
+      </c>
+      <c r="D44" s="6">
+        <v>-0.55301059396834518</v>
+      </c>
+      <c r="E44" s="6">
+        <v>-2.4311866921133549</v>
+      </c>
+      <c r="G44" s="15" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="45" spans="2:7" ht="180" customHeight="1">
+      <c r="B45" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="C45" s="6">
+        <v>-1.3201118976380308</v>
+      </c>
+      <c r="D45" s="6">
+        <v>0.3173555482149748</v>
+      </c>
+      <c r="E45" s="6">
+        <v>-1.0027666204152901</v>
+      </c>
+      <c r="G45" s="15" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="46" spans="2:7" ht="180" customHeight="1">
+      <c r="B46" s="11">
+        <v>0.15</v>
+      </c>
+      <c r="C46" s="6">
+        <v>-0.99269257327984439</v>
+      </c>
+      <c r="D46" s="6">
+        <v>0.91246667958760952</v>
+      </c>
+      <c r="E46" s="6">
+        <v>-7.7459125560157993E-2</v>
+      </c>
+      <c r="G46" s="15" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="47" spans="2:7" ht="180" customHeight="1">
+      <c r="B47" s="11">
+        <v>0.7</v>
+      </c>
+      <c r="C47" s="6">
+        <v>-0.91302850952612324</v>
+      </c>
+      <c r="D47" s="6">
+        <v>-0.14672996852844777</v>
+      </c>
+      <c r="E47" s="6">
+        <v>-1.0597702788743515</v>
+      </c>
+      <c r="G47" s="15" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="48" spans="2:7" ht="180" customHeight="1">
+      <c r="B48" s="11">
+        <v>1.3</v>
+      </c>
+      <c r="C48" s="6">
+        <v>-0.74233228235714854</v>
+      </c>
+      <c r="D48" s="6">
+        <v>-0.21965064164781367</v>
+      </c>
+      <c r="E48" s="6">
+        <v>-0.9619901103319517</v>
+      </c>
+      <c r="G48" s="15" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="49" spans="2:7" ht="180" customHeight="1">
+      <c r="B49" s="11">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="C49" s="6">
+        <v>-0.1216758025375273</v>
+      </c>
+      <c r="D49" s="6">
+        <v>-0.37455260163355697</v>
+      </c>
+      <c r="E49" s="6">
+        <v>-0.49622795613140003</v>
+      </c>
+      <c r="G49" s="15" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="50" spans="2:7" ht="180" customHeight="1">
+      <c r="B50" s="11">
+        <v>0.88</v>
+      </c>
+      <c r="C50" s="6">
+        <v>-0.75893154417661002</v>
+      </c>
+      <c r="D50" s="6">
+        <v>-0.57149399966235848</v>
+      </c>
+      <c r="E50" s="6">
+        <v>-1.3304152914216902</v>
+      </c>
+      <c r="G50" s="15" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="51" spans="2:7" ht="180" customHeight="1">
+      <c r="B51" s="11">
+        <v>0.8</v>
+      </c>
+      <c r="C51" s="6">
+        <v>-0.49620315669371218</v>
+      </c>
+      <c r="D51" s="6">
+        <v>-0.32161652644575844</v>
+      </c>
+      <c r="E51" s="6">
+        <v>-0.81782030299491471</v>
+      </c>
+      <c r="G51" s="15" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="52" spans="2:7" ht="180" customHeight="1">
+      <c r="B52" s="11">
+        <v>1.4</v>
+      </c>
+      <c r="C52" s="6">
+        <v>6.8240716542313784E-3</v>
+      </c>
+      <c r="D52" s="6">
+        <v>-0.53616603732061541</v>
+      </c>
+      <c r="E52" s="6">
+        <v>-0.52934470319236393</v>
+      </c>
+      <c r="G52" s="15" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="53" spans="2:7" ht="180" customHeight="1">
+      <c r="B53" s="11">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="C53" s="6">
+        <v>1.0949404201451522</v>
+      </c>
+      <c r="D53" s="6">
+        <v>-0.57822738232132687</v>
+      </c>
+      <c r="E53" s="6">
+        <v>0.51671460162499905</v>
+      </c>
+      <c r="G53" s="15" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="54" spans="2:7" ht="180" customHeight="1">
+      <c r="B54" s="11">
+        <v>0.6</v>
+      </c>
+      <c r="C54" s="6">
+        <v>-0.51348297413866728</v>
+      </c>
+      <c r="D54" s="6">
+        <v>0.37936876912558581</v>
+      </c>
+      <c r="E54" s="6">
+        <v>-0.13411129411543143</v>
+      </c>
+      <c r="G54" s="15" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="55" spans="2:7" ht="180" customHeight="1">
+      <c r="B55" s="11">
+        <v>0.21</v>
+      </c>
+      <c r="C55" s="6">
+        <v>-0.25009587627974117</v>
+      </c>
+      <c r="D55" s="6">
+        <v>-6.4167102088177774E-2</v>
+      </c>
+      <c r="E55" s="6">
+        <v>-0.31425956558341106</v>
+      </c>
+      <c r="G55" s="15" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="56" spans="2:7" ht="180" customHeight="1">
+      <c r="B56" s="11">
+        <v>0.11</v>
+      </c>
+      <c r="C56" s="6">
+        <v>-1.1568715528486477</v>
+      </c>
+      <c r="D56" s="6">
+        <v>-0.29251414474145143</v>
+      </c>
+      <c r="E56" s="6">
+        <v>-1.4493851744040676</v>
+      </c>
+      <c r="G56" s="15" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="57" spans="2:7" ht="180" customHeight="1">
+      <c r="B57" s="11">
+        <v>0.52</v>
+      </c>
+      <c r="C57" s="6">
+        <v>-0.37825054094607813</v>
+      </c>
+      <c r="D57" s="6">
+        <v>-0.27406812826720239</v>
+      </c>
+      <c r="E57" s="6">
+        <v>-0.65231903733176466</v>
+      </c>
+      <c r="G57" s="15" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="58" spans="2:7" ht="180" customHeight="1">
+      <c r="B58" s="11">
+        <v>0.68</v>
+      </c>
+      <c r="C58" s="6">
+        <v>-1.8426485440571163</v>
+      </c>
+      <c r="D58" s="6">
+        <v>-0.27361924504181045</v>
+      </c>
+      <c r="E58" s="6">
+        <v>-2.1163790816722896</v>
+      </c>
+      <c r="G58" s="15" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="59" spans="2:7" ht="180" customHeight="1">
+      <c r="B59" s="11">
+        <v>0.59</v>
+      </c>
+      <c r="C59" s="6">
+        <v>-0.72634417697301812</v>
+      </c>
+      <c r="D59" s="6">
+        <v>1.4577886281473607E-2</v>
+      </c>
+      <c r="E59" s="6">
+        <v>-0.7117694054479653</v>
+      </c>
+      <c r="G59" s="15" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="60" spans="2:7" ht="180" customHeight="1">
+      <c r="B60" s="11">
+        <v>0.73</v>
+      </c>
+      <c r="C60" s="6">
+        <v>-8.0164925928878361E-2</v>
+      </c>
+      <c r="D60" s="6">
+        <v>-6.5619593348120286E-2</v>
+      </c>
+      <c r="E60" s="6">
+        <v>-0.14578154798368725</v>
+      </c>
+      <c r="G60" s="15" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="61" spans="2:7" ht="180" customHeight="1">
+      <c r="B61" s="11">
+        <v>0.69</v>
+      </c>
+      <c r="C61" s="8"/>
+      <c r="D61" s="8"/>
+      <c r="E61" s="8"/>
+      <c r="G61" s="15" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="62" spans="2:7" ht="180" customHeight="1">
+      <c r="B62" s="11">
+        <v>0.77</v>
+      </c>
+      <c r="C62" s="8"/>
+      <c r="D62" s="8"/>
+      <c r="E62" s="8"/>
+      <c r="G62" s="15" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="63" spans="2:7" ht="180" customHeight="1">
+      <c r="B63" s="11">
+        <v>0.39</v>
+      </c>
+      <c r="C63" s="6">
+        <v>-0.90902576707244931</v>
+      </c>
+      <c r="D63" s="6">
+        <v>-0.32958545611703371</v>
+      </c>
+      <c r="E63" s="6">
+        <v>-1.2386139793506921</v>
+      </c>
+      <c r="G63" s="15" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="64" spans="2:7" ht="180" customHeight="1">
+      <c r="B64" s="11">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C64" s="6">
+        <v>-3.8503743400800872E-2</v>
+      </c>
+      <c r="D64" s="6">
+        <v>-1.0826693492620887E-2</v>
+      </c>
+      <c r="E64" s="6">
+        <v>-4.9328349758112289E-2</v>
+      </c>
+      <c r="G64" s="15" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="65" spans="2:7" ht="180" customHeight="1">
+      <c r="B65" s="11">
+        <v>1.51</v>
+      </c>
+      <c r="C65" s="6">
+        <v>-0.10571903040126651</v>
+      </c>
+      <c r="D65" s="6">
+        <v>6.0529215043047202E-2</v>
+      </c>
+      <c r="E65" s="6">
+        <v>-4.518718337023131E-2</v>
+      </c>
+      <c r="G65" s="15" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="66" spans="2:7" ht="180" customHeight="1">
+      <c r="B66" s="11">
+        <v>0.69</v>
+      </c>
+      <c r="C66" s="6">
+        <v>-0.10823304310544746</v>
+      </c>
+      <c r="D66" s="6">
+        <v>0.15792420239731664</v>
+      </c>
+      <c r="E66" s="6">
+        <v>4.9692160584632106E-2</v>
+      </c>
+      <c r="G66" s="15" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="67" spans="2:7" ht="180" customHeight="1">
+      <c r="B67" s="11">
+        <v>0.08</v>
+      </c>
+      <c r="C67" s="8"/>
+      <c r="D67" s="8"/>
+      <c r="E67" s="8"/>
+      <c r="F67" s="10"/>
+      <c r="G67" s="15" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="68" spans="2:7" ht="180" customHeight="1">
+      <c r="B68" s="11">
+        <v>0.35</v>
+      </c>
+      <c r="C68" s="6">
+        <v>-0.32735893438633035</v>
+      </c>
+      <c r="D68" s="6">
+        <v>-0.25853964718890232</v>
+      </c>
+      <c r="E68" s="6">
+        <v>-0.58589359506374894</v>
+      </c>
+      <c r="G68" s="15" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="69" spans="2:7" ht="180" customHeight="1">
+      <c r="B69" s="11">
+        <v>0.05</v>
+      </c>
+      <c r="C69" s="8"/>
+      <c r="D69" s="8"/>
+      <c r="E69" s="8"/>
+      <c r="G69" s="15" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="70" spans="2:7" ht="180" customHeight="1">
+      <c r="B70" s="11">
+        <v>0.22</v>
+      </c>
+      <c r="C70" s="6">
+        <v>-1.9252629659431351</v>
+      </c>
+      <c r="D70" s="6">
+        <v>9.063094726615617E-2</v>
+      </c>
+      <c r="E70" s="6">
+        <v>-1.8346241726966102</v>
+      </c>
+      <c r="G70" s="15" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="71" spans="2:7" ht="180" customHeight="1">
+      <c r="B71" s="11">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="C71" s="6">
+        <v>-1.4781049346009159</v>
+      </c>
+      <c r="D71" s="6">
+        <v>0.50498135300934122</v>
+      </c>
+      <c r="E71" s="6">
+        <v>-0.9731192512890976</v>
+      </c>
+      <c r="G71" s="15" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="72" spans="2:7" ht="180" customHeight="1">
+      <c r="B72" s="11">
+        <v>0.26</v>
+      </c>
+      <c r="C72" s="6">
+        <v>-1.4036268380538932</v>
+      </c>
+      <c r="D72" s="6">
+        <v>0.22325651254074685</v>
+      </c>
+      <c r="E72" s="6">
+        <v>-1.1803755682145809</v>
+      </c>
+      <c r="G72" s="15" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="73" spans="2:7" ht="180" customHeight="1">
+      <c r="B73" s="11">
+        <v>0.84</v>
+      </c>
+      <c r="C73" s="6">
+        <v>-0.90902576707244931</v>
+      </c>
+      <c r="D73" s="6">
+        <v>-4.7104663356782428E-2</v>
+      </c>
+      <c r="E73" s="6">
+        <v>-0.95611884302475136</v>
+      </c>
+      <c r="G73" s="15" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="74" spans="2:7" ht="180" customHeight="1">
+      <c r="B74" s="11">
+        <v>0</v>
+      </c>
+      <c r="C74" s="8"/>
+      <c r="D74" s="8"/>
+      <c r="E74" s="8"/>
+      <c r="G74" s="15" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="75" spans="2:7" ht="180" customHeight="1">
+      <c r="B75" s="11">
+        <v>0.89</v>
+      </c>
+      <c r="C75" s="6">
+        <v>-3.4230208480657609E-2</v>
+      </c>
+      <c r="D75" s="6">
+        <v>7.4317499528680386E-2</v>
+      </c>
+      <c r="E75" s="6">
+        <v>4.008887009564166E-2</v>
+      </c>
+      <c r="G75" s="15" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="76" spans="2:7" ht="180" customHeight="1">
+      <c r="B76" s="11">
+        <v>0.92</v>
+      </c>
+      <c r="C76" s="6">
+        <v>7.4737034056865159E-2</v>
+      </c>
+      <c r="D76" s="6">
+        <v>-2.5385413663546075E-2</v>
+      </c>
+      <c r="E76" s="6">
+        <v>4.9353543474047079E-2</v>
+      </c>
+      <c r="G76" s="15" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="77" spans="2:7" ht="180" customHeight="1">
+      <c r="B77" s="11">
+        <v>0.7</v>
+      </c>
+      <c r="C77" s="6">
+        <v>-1.1719352992845236</v>
+      </c>
+      <c r="D77" s="6">
+        <v>-0.44352880842387066</v>
+      </c>
+      <c r="E77" s="6">
+        <v>-1.6154460919688214</v>
+      </c>
+      <c r="G77" s="15" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="78" spans="2:7" ht="180" customHeight="1">
+      <c r="B78" s="11">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="C78" s="8"/>
+      <c r="D78" s="8"/>
+      <c r="E78" s="6">
+        <v>-4.9336138120977875</v>
+      </c>
+      <c r="G78" s="15" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="79" spans="2:7" ht="180" customHeight="1">
+      <c r="B79" s="11">
+        <v>0.34</v>
+      </c>
+      <c r="C79" s="6">
+        <v>-2.4693310102934105</v>
+      </c>
+      <c r="D79" s="6">
+        <v>-1.8975046625198111E-2</v>
+      </c>
+      <c r="E79" s="6">
+        <v>-2.4880096088241901</v>
+      </c>
+      <c r="G79" s="15" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="80" spans="2:7" ht="180" customHeight="1">
+      <c r="B80" s="11">
+        <v>0.17</v>
+      </c>
+      <c r="C80" s="6">
+        <v>-2.9464522650130731</v>
+      </c>
+      <c r="D80" s="6">
+        <v>-5.9780251840064302E-2</v>
+      </c>
+      <c r="E80" s="6">
+        <v>-3.0067571031480953</v>
+      </c>
+      <c r="G80" s="15" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="81" spans="2:7" ht="180" customHeight="1">
+      <c r="B81" s="11">
+        <v>0.62</v>
+      </c>
+      <c r="C81" s="6">
+        <v>-0.30696577574448725</v>
+      </c>
+      <c r="D81" s="6">
+        <v>2.7860098289679058E-2</v>
+      </c>
+      <c r="E81" s="6">
+        <v>-0.27910517638973431</v>
+      </c>
+      <c r="G81" s="15" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="82" spans="2:7" ht="180" customHeight="1">
+      <c r="B82" s="11">
+        <v>1.19</v>
+      </c>
+      <c r="C82" s="6">
+        <v>-9.7032851216173555E-2</v>
+      </c>
+      <c r="D82" s="6">
+        <v>-8.8222130202943116E-2</v>
+      </c>
+      <c r="E82" s="6">
+        <v>-0.18525520290728892</v>
+      </c>
+      <c r="G82" s="15" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="83" spans="2:7" ht="180" customHeight="1">
+      <c r="B83" s="11">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="C83" s="6">
+        <v>-2.5662410233014672</v>
+      </c>
+      <c r="D83" s="6">
+        <v>-8.3377360641232912E-2</v>
+      </c>
+      <c r="E83" s="6">
+        <v>-2.6491830782532682</v>
+      </c>
+      <c r="G83" s="15" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="84" spans="2:7" ht="180" customHeight="1">
+      <c r="B84" s="11">
+        <v>0.96</v>
+      </c>
+      <c r="C84" s="6">
+        <v>-3.6454222693490919</v>
+      </c>
+      <c r="D84" s="6">
+        <v>-0.50830085899886401</v>
+      </c>
+      <c r="E84" s="6">
+        <v>-4.1554625617141436</v>
+      </c>
+      <c r="G84" s="15" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="85" spans="2:7" ht="180" customHeight="1">
+      <c r="B85" s="11">
+        <v>0.85</v>
+      </c>
+      <c r="C85" s="6">
+        <v>-2.5150885008540858</v>
+      </c>
+      <c r="D85" s="6">
+        <v>-1.1351480959786329</v>
+      </c>
+      <c r="E85" s="6">
+        <v>-3.6548602111449586</v>
+      </c>
+      <c r="G85" s="15" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="86" spans="2:7" ht="180" customHeight="1">
+      <c r="B86" s="11">
+        <v>1.27</v>
+      </c>
+      <c r="C86" s="8"/>
+      <c r="D86" s="8"/>
+      <c r="E86" s="8"/>
+      <c r="G86" s="15" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="87" spans="2:7" ht="180" customHeight="1">
+      <c r="B87" s="11">
+        <v>1.5</v>
+      </c>
+      <c r="C87" s="8"/>
+      <c r="D87" s="8"/>
+      <c r="E87" s="8"/>
+      <c r="G87" s="15" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="88" spans="2:7" ht="180" customHeight="1">
+      <c r="B88" s="11">
+        <v>0.41</v>
+      </c>
+      <c r="C88" s="6">
+        <v>-0.22135774393160412</v>
+      </c>
+      <c r="D88" s="6">
+        <v>0.20395135734536041</v>
+      </c>
+      <c r="E88" s="6">
+        <v>-1.740471672095012E-2</v>
+      </c>
+      <c r="G88" s="15" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="89" spans="2:7" ht="180" customHeight="1">
+      <c r="B89" s="11">
+        <v>0</v>
+      </c>
+      <c r="C89" s="8"/>
+      <c r="D89" s="8"/>
+      <c r="E89" s="8"/>
+      <c r="G89" s="15" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="90" spans="2:7" ht="180" customHeight="1">
+      <c r="B90" s="11">
+        <v>1.41</v>
+      </c>
+      <c r="C90" s="6">
+        <v>-2.3782505409460781</v>
+      </c>
+      <c r="D90" s="6">
+        <v>-0.26224367375168622</v>
+      </c>
+      <c r="E90" s="6">
+        <v>-2.6402512573863421</v>
+      </c>
+      <c r="G90" s="15" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="91" spans="2:7" ht="180" customHeight="1">
+      <c r="B91" s="11">
+        <v>0</v>
+      </c>
+      <c r="C91" s="8"/>
+      <c r="D91" s="8"/>
+      <c r="E91" s="8"/>
+      <c r="G91" s="15" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="92" spans="2:7" ht="180" customHeight="1">
+      <c r="B92" s="11">
+        <v>0.27</v>
+      </c>
+      <c r="C92" s="6">
+        <v>-1.3542755076172064</v>
+      </c>
+      <c r="D92" s="6">
+        <v>-0.82094714995130658</v>
+      </c>
+      <c r="E92" s="6">
+        <v>-2.1750803898605011</v>
+      </c>
+      <c r="G92" s="15" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="93" spans="2:7" ht="180" customHeight="1">
+      <c r="B93" s="11">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="C93" s="8"/>
+      <c r="D93" s="8"/>
+      <c r="E93" s="6">
+        <v>-4.53567380342575</v>
+      </c>
+      <c r="G93" s="15" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="94" spans="2:7" ht="180" customHeight="1">
+      <c r="B94" s="11">
+        <v>0.13</v>
+      </c>
+      <c r="C94" s="6">
+        <v>-1.8895474136766004</v>
+      </c>
+      <c r="D94" s="6">
+        <v>-0.16957742772938156</v>
+      </c>
+      <c r="E94" s="6">
+        <v>-2.0591319943983213</v>
+      </c>
+      <c r="G94" s="15" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="95" spans="2:7" ht="180" customHeight="1">
+      <c r="B95" s="11">
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="C95" s="6">
+        <v>-1.2518470660795045</v>
+      </c>
+      <c r="D95" s="6">
+        <v>-0.33351574974546616</v>
+      </c>
+      <c r="E95" s="6">
+        <v>-1.5854063354121615</v>
+      </c>
+      <c r="G95" s="15" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="96" spans="2:7" ht="180" customHeight="1">
+      <c r="B96" s="11">
+        <v>0.1</v>
+      </c>
+      <c r="C96" s="8"/>
+      <c r="D96" s="8"/>
+      <c r="E96" s="8"/>
+      <c r="G96" s="15" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="97" spans="2:7" ht="180" customHeight="1">
+      <c r="B97" s="11">
+        <v>0</v>
+      </c>
+      <c r="C97" s="8"/>
+      <c r="D97" s="8"/>
+      <c r="E97" s="8"/>
+      <c r="G97" s="15" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="98" spans="2:7" ht="180" customHeight="1">
+      <c r="B98" s="11">
+        <v>0</v>
+      </c>
+      <c r="C98" s="8"/>
+      <c r="D98" s="8"/>
+      <c r="E98" s="8"/>
+      <c r="G98" s="15" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="99" spans="2:7" ht="180" customHeight="1">
+      <c r="B99" s="11">
+        <v>0.1</v>
+      </c>
+      <c r="C99" s="8"/>
+      <c r="D99" s="8"/>
+      <c r="E99" s="8"/>
+      <c r="G99" s="15" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="100" spans="2:7" ht="180" customHeight="1">
+      <c r="B100" s="11">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="C100" s="6">
+        <v>-2.4765789529471061E-2</v>
+      </c>
+      <c r="D100" s="6">
+        <v>0.2464243775927728</v>
+      </c>
+      <c r="E100" s="6">
+        <v>0.22165996190507276</v>
+      </c>
+      <c r="G100" s="15" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="101" spans="2:7" ht="180" customHeight="1">
+      <c r="B101" s="11">
+        <v>0.53</v>
+      </c>
+      <c r="C101" s="6">
+        <v>-2.8325089127062362</v>
+      </c>
+      <c r="D101" s="6">
+        <v>-0.50830085899886401</v>
+      </c>
+      <c r="E101" s="6">
+        <v>-3.3425492050712884</v>
+      </c>
+      <c r="G101" s="15" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="102" spans="2:7" ht="180" customHeight="1">
+      <c r="B102" s="11">
+        <v>1.08</v>
+      </c>
+      <c r="C102" s="6">
+        <v>-0.13621974701798889</v>
+      </c>
+      <c r="D102" s="6">
+        <v>-0.10773670650067757</v>
+      </c>
+      <c r="E102" s="6">
+        <v>-0.24395428411410158</v>
+      </c>
+      <c r="G102" s="15" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="103" spans="2:7" ht="180" customHeight="1">
+      <c r="B103" s="12">
+        <v>1</v>
+      </c>
+      <c r="C103" s="6">
+        <v>0</v>
+      </c>
+      <c r="D103" s="6">
+        <v>0</v>
+      </c>
+      <c r="E103" s="6">
+        <v>0</v>
+      </c>
+      <c r="G103" s="15" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="104" spans="2:7" ht="180" customHeight="1">
+      <c r="B104" s="11"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <conditionalFormatting sqref="C2:E1048576">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="num" val="-5"/>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color rgb="FF00305B"/>
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+        <color rgb="FFCCA11B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I2:I8">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="num" val="-5"/>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color rgb="FF00305B"/>
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+        <color rgb="FFCCA11B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1:B1048576">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="between">
+      <formula>0.8</formula>
+      <formula>2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="between">
+      <formula>0.11</formula>
+      <formula>0.79</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="between">
+      <formula>0</formula>
+      <formula>0.1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
+  <pageSetup paperSize="58" scale="10" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="10"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Presubmission version of manuscript
</commit_message>
<xml_diff>
--- a/draft/fig2/heatmap.xlsx
+++ b/draft/fig2/heatmap.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2620" yWindow="0" windowWidth="33740" windowHeight="21140" tabRatio="500" activeTab="5"/>
+    <workbookView xWindow="2620" yWindow="0" windowWidth="33740" windowHeight="21140" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -926,41 +926,7 @@
     <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="1" tint="0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <strike/>
@@ -993,6 +959,664 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet4!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>kcat/km</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet4!$D$15:$D$97</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="83"/>
+                <c:pt idx="0">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.7</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6.7</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11.7</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4.6</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>12.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>84.1</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>39.1</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>12.7</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>11.4</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>10.5</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>59.5</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>49.5</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>25.8</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>61.6</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>197.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>154.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>143.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>109.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>26.5</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>154.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>34.9</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>113.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>108.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>42.3</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>29.4</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>160.0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>109.0</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>123.0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>199.0</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>282.0</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>472.0</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>479.0</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>166.0</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>370.0</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>320.0</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>405.0</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>416.0</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>848.0</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>898.0</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>668.0</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>464.0</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>807.0</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>497.0</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>687.0</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>547.0</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>641.0</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>670.0</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>555.0</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>436.0</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>646.0</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>1060.0</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>504.0</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>707.0</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>613.0</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>800.0</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>403.0</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>735.0</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>271.0</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>846.0</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>89.9</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>809.0</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>693.0</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>986.0</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>531.0</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>695.0</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>884.0</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>946.0</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>817.0</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>1050.0</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>689.0</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>801.0</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>878.0</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>835.0</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>1470.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet4!$G$15:$G$97</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="83"/>
+                <c:pt idx="0">
+                  <c:v>12.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>38.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>78.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>82.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>169.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>193.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>198.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>385.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>393.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>558.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>563.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>636.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>713.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>789.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>943.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1147.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1313.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1498.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2512.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>4161.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>4459.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>4760.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>6099.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>6254.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>8021.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>9470.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>9909.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>10600.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>11000.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>11331.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>14733.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>14958.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>17056.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>18261.0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>18735.0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>18990.0</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>23930.0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>25286.0</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>26111.0</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>29317.0</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>32808.0</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>33333.0</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>38223.0</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>38788.0</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>39320.0</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>44540.0</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>45838.0</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>50734.0</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>54754.0</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>71275.0</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>72703.0</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>83250.0</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>83273.0</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>87520.0</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>87568.0</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>89572.0</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>89661.0</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>90269.0</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>97879.0</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>100000.0</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>102439.0</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>112044.0</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>112066.0</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>114943.0</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>119940.0</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>122705.0</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>126047.0</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>126080.0</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>143610.0</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>153220.0</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>154688.0</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>164883.0</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>164907.0</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>168281.0</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>171650.0</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>185855.0</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>188249.0</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>192308.0</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>192458.0</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>223120.0</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>253757.0</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>285959.0</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>337931.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2101570376"/>
+        <c:axId val="2101566680"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="2101570376"/>
+        <c:scaling>
+          <c:logBase val="10.0"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2101566680"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2101566680"/>
+        <c:scaling>
+          <c:logBase val="10.0"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2101570376"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>69850</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>723900</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3323,8 +3947,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H106"/>
   <sheetViews>
-    <sheetView topLeftCell="A71" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6090,6 +6714,7 @@
     <sortCondition ref="G1"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -7472,7 +8097,7 @@
   </sheetPr>
   <dimension ref="B1:Y104"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A82" zoomScale="16" zoomScaleNormal="16" zoomScalePageLayoutView="16" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A77" zoomScale="16" zoomScaleNormal="16" zoomScalePageLayoutView="16" workbookViewId="0">
       <selection activeCell="W13" sqref="W13"/>
     </sheetView>
   </sheetViews>
@@ -9195,11 +9820,11 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="cellIs" dxfId="4" priority="4" operator="between">
+    <cfRule type="cellIs" dxfId="1" priority="4" operator="between">
       <formula>0</formula>
       <formula>0.1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="between">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="between">
       <formula>0.11</formula>
       <formula>2</formula>
     </cfRule>

</xml_diff>

<commit_message>
Added cleaned versions of draft and supplemental
</commit_message>
<xml_diff>
--- a/draft/fig2/heatmap.xlsx
+++ b/draft/fig2/heatmap.xlsx
@@ -976,6 +976,26 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>kcat versus</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> km</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
     </c:title>
@@ -1264,258 +1284,258 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet4!$G$15:$G$97</c:f>
+              <c:f>Sheet4!$E$15:$E$97</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="83"/>
                 <c:pt idx="0">
-                  <c:v>12.0</c:v>
+                  <c:v>0.0166</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>38.0</c:v>
+                  <c:v>0.0703</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>78.0</c:v>
+                  <c:v>0.0166</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>82.0</c:v>
+                  <c:v>0.0232</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>169.0</c:v>
+                  <c:v>0.00591</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>193.0</c:v>
+                  <c:v>0.0135</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>198.0</c:v>
+                  <c:v>0.00101</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>385.0</c:v>
+                  <c:v>0.00624</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>393.0</c:v>
+                  <c:v>0.00942</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>558.0</c:v>
+                  <c:v>0.00538</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>563.0</c:v>
+                  <c:v>0.0119</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>636.0</c:v>
+                  <c:v>0.0184</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>713.0</c:v>
+                  <c:v>0.00645</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>789.0</c:v>
+                  <c:v>0.0152</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>943.0</c:v>
+                  <c:v>0.0892</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1147.0</c:v>
+                  <c:v>0.0341</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1313.0</c:v>
+                  <c:v>0.00967</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1498.0</c:v>
+                  <c:v>0.00761</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2512.0</c:v>
+                  <c:v>0.00418</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>4161.0</c:v>
+                  <c:v>0.0143</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>4459.0</c:v>
+                  <c:v>0.0111</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>4760.0</c:v>
+                  <c:v>0.00542</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>6099.0</c:v>
+                  <c:v>0.0101</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>6254.0</c:v>
+                  <c:v>0.0315</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>8021.0</c:v>
+                  <c:v>0.0192</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>9470.0</c:v>
+                  <c:v>0.0151</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>9909.0</c:v>
+                  <c:v>0.011</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>10600.0</c:v>
+                  <c:v>0.0025</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>11000.0</c:v>
+                  <c:v>0.014</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>11331.0</c:v>
+                  <c:v>0.00308</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>14733.0</c:v>
+                  <c:v>0.00767</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>14958.0</c:v>
+                  <c:v>0.00722</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>17056.0</c:v>
+                  <c:v>0.00248</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>18261.0</c:v>
+                  <c:v>0.00161</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>18735.0</c:v>
+                  <c:v>0.00854</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>18990.0</c:v>
+                  <c:v>0.00574</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>23930.0</c:v>
+                  <c:v>0.00514</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>25286.0</c:v>
+                  <c:v>0.00787</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>26111.0</c:v>
+                  <c:v>0.0108</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>29317.0</c:v>
+                  <c:v>0.0161</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>32808.0</c:v>
+                  <c:v>0.0146</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>33333.0</c:v>
+                  <c:v>0.00498</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>38223.0</c:v>
+                  <c:v>0.00968</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>38788.0</c:v>
+                  <c:v>0.00825</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>39320.0</c:v>
+                  <c:v>0.0103</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>44540.0</c:v>
+                  <c:v>0.00934</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>45838.0</c:v>
+                  <c:v>0.0185</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>50734.0</c:v>
+                  <c:v>0.0177</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>54754.0</c:v>
+                  <c:v>0.0122</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>71275.0</c:v>
+                  <c:v>0.00651</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>72703.0</c:v>
+                  <c:v>0.0111</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>83250.0</c:v>
+                  <c:v>0.00597</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>83273.0</c:v>
+                  <c:v>0.00825</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>87520.0</c:v>
+                  <c:v>0.00625</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>87568.0</c:v>
+                  <c:v>0.00732</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>89572.0</c:v>
+                  <c:v>0.00748</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>89661.0</c:v>
+                  <c:v>0.00619</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>90269.0</c:v>
+                  <c:v>0.00483</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>97879.0</c:v>
+                  <c:v>0.0066</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>100000.0</c:v>
+                  <c:v>0.0106</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>102439.0</c:v>
+                  <c:v>0.00492</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>112044.0</c:v>
+                  <c:v>0.00631</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>112066.0</c:v>
+                  <c:v>0.00547</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>114943.0</c:v>
+                  <c:v>0.00696</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>119940.0</c:v>
+                  <c:v>0.00336</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>122705.0</c:v>
+                  <c:v>0.00599</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>126047.0</c:v>
+                  <c:v>0.00215</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>126080.0</c:v>
+                  <c:v>0.00671</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>143610.0</c:v>
+                  <c:v>0.00063</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>153220.0</c:v>
+                  <c:v>0.00528</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>154688.0</c:v>
+                  <c:v>0.00448</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>164883.0</c:v>
+                  <c:v>0.00598</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>164907.0</c:v>
+                  <c:v>0.00322</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>168281.0</c:v>
+                  <c:v>0.00413</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>171650.0</c:v>
+                  <c:v>0.00515</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>185855.0</c:v>
+                  <c:v>0.00509</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>188249.0</c:v>
+                  <c:v>0.00434</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>192308.0</c:v>
+                  <c:v>0.00546</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>192458.0</c:v>
+                  <c:v>0.00358</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>223120.0</c:v>
+                  <c:v>0.00359</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>253757.0</c:v>
+                  <c:v>0.00346</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>285959.0</c:v>
+                  <c:v>0.00292</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>337931.0</c:v>
+                  <c:v>0.00435</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1530,11 +1550,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2101570376"/>
-        <c:axId val="2101566680"/>
+        <c:axId val="2090604952"/>
+        <c:axId val="2090607912"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2101570376"/>
+        <c:axId val="2090604952"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -1545,12 +1565,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2101566680"/>
+        <c:crossAx val="2090607912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2101566680"/>
+        <c:axId val="2090607912"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -1562,7 +1582,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2101570376"/>
+        <c:crossAx val="2090604952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3947,8 +3967,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H106"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="U23" sqref="U23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>